<commit_message>
fixing formatting and other issues identified with linting
</commit_message>
<xml_diff>
--- a/examples/sbtab/SBtab.xlsx
+++ b/examples/sbtab/SBtab.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="12330"/>
+    <workbookView windowWidth="21990" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Schema" sheetId="1" r:id="rId1"/>
@@ -1198,7 +1198,7 @@
     <t>Relation</t>
   </si>
   <si>
-    <t>from</t>
+    <t>from_object</t>
   </si>
   <si>
     <t>Element at beginning of arrow</t>
@@ -1213,7 +1213,7 @@
     <t>Flag indicating non-symmetric relations</t>
   </si>
   <si>
-    <t>to</t>
+    <t>to_object</t>
   </si>
   <si>
     <t>Element at arrowhead</t>
@@ -1406,7 +1406,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1428,52 +1428,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -1486,6 +1440,28 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1513,6 +1489,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -1520,7 +1527,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1536,17 +1549,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1557,23 +1564,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1600,7 +1593,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1612,19 +1623,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1636,79 +1689,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1726,19 +1719,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1750,31 +1737,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1794,26 +1787,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1825,6 +1798,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1854,21 +1836,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1885,157 +1852,183 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2373,9 +2366,9 @@
   <dimension ref="A1:G438"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A387" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A395" sqref="A395"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelCol="6"/>

</xml_diff>